<commit_message>
tabs added for reminders strategy to be measured sessions 11-13
</commit_message>
<xml_diff>
--- a/data/KAHI_strategy.xlsx
+++ b/data/KAHI_strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8B85E7-8F83-C643-97BC-F708A4EF7DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8AC9D5-B146-5E4B-B5CC-670802486732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35240" yWindow="6780" windowWidth="27640" windowHeight="15920" xr2:uid="{422B1A0C-E1E2-D844-A423-453C58228ACE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>session</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>help</t>
+  </si>
+  <si>
+    <t>freq_2</t>
+  </si>
+  <si>
+    <t>help_2</t>
   </si>
 </sst>
 </file>
@@ -393,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB64791-6C28-004E-A47E-B88BDB5885C0}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +417,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>7</v>
       </c>
@@ -423,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8</v>
       </c>
@@ -434,7 +446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9</v>
       </c>
@@ -445,7 +457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>

</xml_diff>